<commit_message>
Added Tasks and Tests
Also updated Functions, Features, and Constraints list
</commit_message>
<xml_diff>
--- a/Design/Views.xlsx
+++ b/Design/Views.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22604"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22620"/>
   <workbookPr defaultThemeVersion="166925"/>
   <xr:revisionPtr revIDLastSave="37" documentId="11_D35B414544ABFA6AB65D92491572BF502C73FDF8" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FDD4D2A4-2FDB-473A-96D4-2CF3DBCF2576}"/>
   <bookViews>
@@ -424,7 +424,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -523,6 +523,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DC88C5F7ED967241B3C1B23F7D8FE943" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0500d2a4d189bfd2cd95983d6486ec91">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b6a19767-1883-4ae5-86d0-5dd274dd8983" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="51cc84d281eae70be64b1fb4808b6790" ns2:_="">
     <xsd:import namespace="b6a19767-1883-4ae5-86d0-5dd274dd8983"/>
@@ -706,15 +715,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -722,11 +722,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9226A648-D950-4103-9212-66D93F17E5DC}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F0F38EF-DB00-4D94-BE00-38B90B89EC5F}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9226A648-D950-4103-9212-66D93F17E5DC}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>